<commit_message>
finish process excel data
</commit_message>
<xml_diff>
--- a/resources/questions.xlsx
+++ b/resources/questions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>狐假虎威</t>
   </si>
@@ -88,13 +88,6 @@
       </rPr>
       <t>巢</t>
     </r>
-  </si>
-  <si>
-    <t>答案</t>
-    <rPh sb="0" eb="2">
-      <t>da'a</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>选项序号</t>
@@ -293,7 +286,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -307,9 +300,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -632,27 +622,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" customWidth="1"/>
-    <col min="6" max="6" width="73.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="73.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -661,173 +651,150 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <v>1</v>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2">
+      <c r="D7" s="2">
         <v>2</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="2">
-        <v>1</v>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2">
+      <c r="D9" s="2">
         <v>2</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D2:D3"/>
+  <mergeCells count="12">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>

</xml_diff>